<commit_message>
--newapproxmatch and --oldapproxmatch for which author to pass through in approx match
</commit_message>
<xml_diff>
--- a/ReadAmazonKindleList/example_KindleBooks_Favorites.xlsx
+++ b/ReadAmazonKindleList/example_KindleBooks_Favorites.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub-Mark-MDO47\MDOpythonUtils\ReadAmazonKindleList\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{984B7FCA-8663-4669-B165-2A14C86A80F5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F45B7CFF-0C0B-4315-B179-38E6C9A2B8E5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1830" yWindow="3390" windowWidth="28800" windowHeight="10545" xr2:uid="{0BC05AE5-A058-4C1D-AAC0-1427022E5248}"/>
+    <workbookView xWindow="8415" yWindow="4560" windowWidth="28800" windowHeight="10545" activeTab="2" xr2:uid="{0BC05AE5-A058-4C1D-AAC0-1427022E5248}"/>
   </bookViews>
   <sheets>
     <sheet name="Books" sheetId="4" r:id="rId1"/>
@@ -287,7 +287,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -299,6 +299,7 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Check Cell" xfId="1" builtinId="23"/>
@@ -614,11 +615,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{10CDE8BA-1414-4B51-8A6F-644E810BC2AB}">
-  <dimension ref="A1:H13"/>
+  <dimension ref="A1:H29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C15" sqref="C15"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E2" sqref="E2:E29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -669,7 +670,7 @@
       <c r="D2" t="s">
         <v>37</v>
       </c>
-      <c r="E2">
+      <c r="E2" s="5">
         <v>1</v>
       </c>
       <c r="F2" t="s">
@@ -686,6 +687,7 @@
       <c r="C3" t="s">
         <v>6</v>
       </c>
+      <c r="E3" s="5"/>
       <c r="F3" t="s">
         <v>34</v>
       </c>
@@ -703,7 +705,7 @@
       <c r="D4" t="s">
         <v>42</v>
       </c>
-      <c r="E4">
+      <c r="E4" s="5">
         <v>1</v>
       </c>
     </row>
@@ -720,7 +722,7 @@
       <c r="D5" t="s">
         <v>40</v>
       </c>
-      <c r="E5">
+      <c r="E5" s="5">
         <v>1</v>
       </c>
     </row>
@@ -734,6 +736,7 @@
       <c r="C6" t="s">
         <v>12</v>
       </c>
+      <c r="E6" s="5"/>
     </row>
     <row r="7" spans="1:8">
       <c r="A7" t="s">
@@ -745,6 +748,7 @@
       <c r="C7" t="s">
         <v>14</v>
       </c>
+      <c r="E7" s="5"/>
     </row>
     <row r="8" spans="1:8">
       <c r="A8" t="s">
@@ -756,6 +760,7 @@
       <c r="C8" t="s">
         <v>16</v>
       </c>
+      <c r="E8" s="5"/>
     </row>
     <row r="9" spans="1:8">
       <c r="A9" t="s">
@@ -767,6 +772,7 @@
       <c r="C9" t="s">
         <v>18</v>
       </c>
+      <c r="E9" s="5"/>
       <c r="F9" t="s">
         <v>36</v>
       </c>
@@ -784,7 +790,7 @@
       <c r="D10" t="s">
         <v>19</v>
       </c>
-      <c r="E10">
+      <c r="E10" s="5">
         <v>1</v>
       </c>
     </row>
@@ -801,7 +807,7 @@
       <c r="D11" t="s">
         <v>19</v>
       </c>
-      <c r="E11">
+      <c r="E11" s="5">
         <v>2</v>
       </c>
     </row>
@@ -818,7 +824,7 @@
       <c r="D12" t="s">
         <v>39</v>
       </c>
-      <c r="E12">
+      <c r="E12" s="5">
         <v>1</v>
       </c>
     </row>
@@ -832,9 +838,58 @@
       <c r="C13" t="s">
         <v>23</v>
       </c>
+      <c r="E13" s="5"/>
       <c r="H13" t="s">
         <v>38</v>
       </c>
+    </row>
+    <row r="14" spans="1:8">
+      <c r="E14" s="5"/>
+    </row>
+    <row r="15" spans="1:8">
+      <c r="E15" s="5"/>
+    </row>
+    <row r="16" spans="1:8">
+      <c r="E16" s="5"/>
+    </row>
+    <row r="17" spans="5:5">
+      <c r="E17" s="5"/>
+    </row>
+    <row r="18" spans="5:5">
+      <c r="E18" s="5"/>
+    </row>
+    <row r="19" spans="5:5">
+      <c r="E19" s="5"/>
+    </row>
+    <row r="20" spans="5:5">
+      <c r="E20" s="5"/>
+    </row>
+    <row r="21" spans="5:5">
+      <c r="E21" s="5"/>
+    </row>
+    <row r="22" spans="5:5">
+      <c r="E22" s="5"/>
+    </row>
+    <row r="23" spans="5:5">
+      <c r="E23" s="5"/>
+    </row>
+    <row r="24" spans="5:5">
+      <c r="E24" s="5"/>
+    </row>
+    <row r="25" spans="5:5">
+      <c r="E25" s="5"/>
+    </row>
+    <row r="26" spans="5:5">
+      <c r="E26" s="5"/>
+    </row>
+    <row r="27" spans="5:5">
+      <c r="E27" s="5"/>
+    </row>
+    <row r="28" spans="5:5">
+      <c r="E28" s="5"/>
+    </row>
+    <row r="29" spans="5:5">
+      <c r="E29" s="5"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:H13" xr:uid="{30F64046-9FAB-4BA1-AF8F-52353D1AAE75}"/>
@@ -850,10 +905,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DA8C6A36-94C2-4C7F-8CA3-6F5CB9421129}">
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:E26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6:XFD13"/>
+      <selection activeCell="C2" sqref="C2:C26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -884,7 +939,7 @@
       <c r="B2" t="s">
         <v>43</v>
       </c>
-      <c r="C2">
+      <c r="C2" s="5">
         <v>1</v>
       </c>
       <c r="E2" s="4" t="s">
@@ -898,7 +953,7 @@
       <c r="B3" t="s">
         <v>43</v>
       </c>
-      <c r="C3">
+      <c r="C3" s="5">
         <v>2</v>
       </c>
     </row>
@@ -909,7 +964,7 @@
       <c r="B4" t="s">
         <v>19</v>
       </c>
-      <c r="C4">
+      <c r="C4" s="5">
         <v>1</v>
       </c>
     </row>
@@ -920,9 +975,72 @@
       <c r="B5" t="s">
         <v>19</v>
       </c>
-      <c r="C5">
+      <c r="C5" s="5">
         <v>2</v>
       </c>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="C6" s="5"/>
+    </row>
+    <row r="7" spans="1:5">
+      <c r="C7" s="5"/>
+    </row>
+    <row r="8" spans="1:5">
+      <c r="C8" s="5"/>
+    </row>
+    <row r="9" spans="1:5">
+      <c r="C9" s="5"/>
+    </row>
+    <row r="10" spans="1:5">
+      <c r="C10" s="5"/>
+    </row>
+    <row r="11" spans="1:5">
+      <c r="C11" s="5"/>
+    </row>
+    <row r="12" spans="1:5">
+      <c r="C12" s="5"/>
+    </row>
+    <row r="13" spans="1:5">
+      <c r="C13" s="5"/>
+    </row>
+    <row r="14" spans="1:5">
+      <c r="C14" s="5"/>
+    </row>
+    <row r="15" spans="1:5">
+      <c r="C15" s="5"/>
+    </row>
+    <row r="16" spans="1:5">
+      <c r="C16" s="5"/>
+    </row>
+    <row r="17" spans="3:3">
+      <c r="C17" s="5"/>
+    </row>
+    <row r="18" spans="3:3">
+      <c r="C18" s="5"/>
+    </row>
+    <row r="19" spans="3:3">
+      <c r="C19" s="5"/>
+    </row>
+    <row r="20" spans="3:3">
+      <c r="C20" s="5"/>
+    </row>
+    <row r="21" spans="3:3">
+      <c r="C21" s="5"/>
+    </row>
+    <row r="22" spans="3:3">
+      <c r="C22" s="5"/>
+    </row>
+    <row r="23" spans="3:3">
+      <c r="C23" s="5"/>
+    </row>
+    <row r="24" spans="3:3">
+      <c r="C24" s="5"/>
+    </row>
+    <row r="25" spans="3:3">
+      <c r="C25" s="5"/>
+    </row>
+    <row r="26" spans="3:3">
+      <c r="C26" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -931,10 +1049,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{21C572CC-F93B-43EE-89A4-E9C581F676FC}">
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:E19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:C3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -965,7 +1083,7 @@
       <c r="B2" t="s">
         <v>54</v>
       </c>
-      <c r="C2">
+      <c r="C2" s="5">
         <v>1</v>
       </c>
       <c r="E2" s="4" t="s">
@@ -979,9 +1097,57 @@
       <c r="B3" t="s">
         <v>55</v>
       </c>
-      <c r="C3">
+      <c r="C3" s="5">
         <v>1</v>
       </c>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="C4" s="5"/>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="C5" s="5"/>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="C6" s="5"/>
+    </row>
+    <row r="7" spans="1:5">
+      <c r="C7" s="5"/>
+    </row>
+    <row r="8" spans="1:5">
+      <c r="C8" s="5"/>
+    </row>
+    <row r="9" spans="1:5">
+      <c r="C9" s="5"/>
+    </row>
+    <row r="10" spans="1:5">
+      <c r="C10" s="5"/>
+    </row>
+    <row r="11" spans="1:5">
+      <c r="C11" s="5"/>
+    </row>
+    <row r="12" spans="1:5">
+      <c r="C12" s="5"/>
+    </row>
+    <row r="13" spans="1:5">
+      <c r="C13" s="5"/>
+    </row>
+    <row r="14" spans="1:5">
+      <c r="C14" s="5"/>
+    </row>
+    <row r="15" spans="1:5">
+      <c r="C15" s="5"/>
+    </row>
+    <row r="16" spans="1:5">
+      <c r="C16" s="5"/>
+    </row>
+    <row r="17" spans="3:3">
+      <c r="C17" s="5"/>
+    </row>
+    <row r="18" spans="3:3">
+      <c r="C18" s="5"/>
+    </row>
+    <row r="19" spans="3:3">
+      <c r="C19" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
complete code for AcqDate
</commit_message>
<xml_diff>
--- a/ReadAmazonKindleList/example_KindleBooks_Favorites.xlsx
+++ b/ReadAmazonKindleList/example_KindleBooks_Favorites.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub-Mark-MDO47\MDOpythonUtils\ReadAmazonKindleList\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F45B7CFF-0C0B-4315-B179-38E6C9A2B8E5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7CED161D-0426-4E69-8A9A-93E6433CDD1E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8415" yWindow="4560" windowWidth="28800" windowHeight="10545" activeTab="2" xr2:uid="{0BC05AE5-A058-4C1D-AAC0-1427022E5248}"/>
+    <workbookView xWindow="8415" yWindow="4560" windowWidth="28800" windowHeight="10545" xr2:uid="{0BC05AE5-A058-4C1D-AAC0-1427022E5248}"/>
   </bookViews>
   <sheets>
     <sheet name="Books" sheetId="4" r:id="rId1"/>
@@ -18,7 +18,7 @@
     <sheet name="TITLE_partialMatch" sheetId="9" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Books!$A$1:$H$13</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Books!$A$1:$I$13</definedName>
   </definedNames>
   <calcPr calcId="181029"/>
   <extLst>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="59">
   <si>
     <t>Title</t>
   </si>
@@ -204,12 +204,18 @@
   </si>
   <si>
     <t># [lcstring, series, seriesNum</t>
+  </si>
+  <si>
+    <t>DateAcq</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="165" formatCode="mm/dd/yy;@"/>
+  </numFmts>
   <fonts count="4">
     <font>
       <sz val="11"/>
@@ -287,7 +293,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -300,6 +306,7 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Check Cell" xfId="1" builtinId="23"/>
@@ -615,11 +622,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{10CDE8BA-1414-4B51-8A6F-644E810BC2AB}">
-  <dimension ref="A1:H29"/>
+  <dimension ref="A1:I29"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E2" sqref="E2:E29"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -628,10 +635,11 @@
     <col min="2" max="2" width="26.85546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="26.28515625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="30.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="5.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="16.5" thickTop="1" thickBot="1">
+    <row r="1" spans="1:9" ht="16.5" thickTop="1" thickBot="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -648,16 +656,19 @@
         <v>3</v>
       </c>
       <c r="F1" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="15.75" thickTop="1">
+    <row r="2" spans="1:9" ht="15.75" thickTop="1">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -673,11 +684,14 @@
       <c r="E2" s="5">
         <v>1</v>
       </c>
-      <c r="F2" t="s">
+      <c r="F2" s="6">
+        <v>43724</v>
+      </c>
+      <c r="G2" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="3" spans="1:8">
+    <row r="3" spans="1:9">
       <c r="A3" t="s">
         <v>41</v>
       </c>
@@ -688,11 +702,14 @@
         <v>6</v>
       </c>
       <c r="E3" s="5"/>
-      <c r="F3" t="s">
+      <c r="F3" s="6">
+        <v>43907</v>
+      </c>
+      <c r="G3" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="4" spans="1:8">
+    <row r="4" spans="1:9">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -708,8 +725,11 @@
       <c r="E4" s="5">
         <v>1</v>
       </c>
-    </row>
-    <row r="5" spans="1:8">
+      <c r="F4" s="6">
+        <v>44010</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9">
       <c r="A5" t="s">
         <v>9</v>
       </c>
@@ -725,8 +745,11 @@
       <c r="E5" s="5">
         <v>1</v>
       </c>
-    </row>
-    <row r="6" spans="1:8">
+      <c r="F5" s="6">
+        <v>43985</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9">
       <c r="A6" t="s">
         <v>11</v>
       </c>
@@ -737,8 +760,11 @@
         <v>12</v>
       </c>
       <c r="E6" s="5"/>
-    </row>
-    <row r="7" spans="1:8">
+      <c r="F6" s="6">
+        <v>41670</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9">
       <c r="A7" t="s">
         <v>13</v>
       </c>
@@ -749,8 +775,11 @@
         <v>14</v>
       </c>
       <c r="E7" s="5"/>
-    </row>
-    <row r="8" spans="1:8">
+      <c r="F7" s="6">
+        <v>43786</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9">
       <c r="A8" t="s">
         <v>15</v>
       </c>
@@ -761,8 +790,11 @@
         <v>16</v>
       </c>
       <c r="E8" s="5"/>
-    </row>
-    <row r="9" spans="1:8">
+      <c r="F8" s="6">
+        <v>43793</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9">
       <c r="A9" t="s">
         <v>17</v>
       </c>
@@ -773,11 +805,14 @@
         <v>18</v>
       </c>
       <c r="E9" s="5"/>
-      <c r="F9" t="s">
+      <c r="F9" s="6">
+        <v>43652</v>
+      </c>
+      <c r="G9" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="10" spans="1:8">
+    <row r="10" spans="1:9">
       <c r="A10" t="s">
         <v>19</v>
       </c>
@@ -793,8 +828,11 @@
       <c r="E10" s="5">
         <v>1</v>
       </c>
-    </row>
-    <row r="11" spans="1:8">
+      <c r="F10" s="6">
+        <v>43730</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9">
       <c r="A11" t="s">
         <v>21</v>
       </c>
@@ -810,8 +848,11 @@
       <c r="E11" s="5">
         <v>2</v>
       </c>
-    </row>
-    <row r="12" spans="1:8">
+      <c r="F11" s="6">
+        <v>43723</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9">
       <c r="A12" t="s">
         <v>24</v>
       </c>
@@ -827,8 +868,11 @@
       <c r="E12" s="5">
         <v>1</v>
       </c>
-    </row>
-    <row r="13" spans="1:8">
+      <c r="F12" s="6">
+        <v>43532</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9">
       <c r="A13" t="s">
         <v>22</v>
       </c>
@@ -839,66 +883,79 @@
         <v>23</v>
       </c>
       <c r="E13" s="5"/>
-      <c r="H13" t="s">
+      <c r="F13" s="6">
+        <v>43532</v>
+      </c>
+      <c r="I13" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="14" spans="1:8">
+    <row r="14" spans="1:9">
       <c r="E14" s="5"/>
-    </row>
-    <row r="15" spans="1:8">
+      <c r="F14" s="5"/>
+    </row>
+    <row r="15" spans="1:9">
       <c r="E15" s="5"/>
-    </row>
-    <row r="16" spans="1:8">
+      <c r="F15" s="5"/>
+    </row>
+    <row r="16" spans="1:9">
       <c r="E16" s="5"/>
-    </row>
-    <row r="17" spans="5:5">
+      <c r="F16" s="5"/>
+    </row>
+    <row r="17" spans="5:6">
       <c r="E17" s="5"/>
-    </row>
-    <row r="18" spans="5:5">
+      <c r="F17" s="5"/>
+    </row>
+    <row r="18" spans="5:6">
       <c r="E18" s="5"/>
-    </row>
-    <row r="19" spans="5:5">
+      <c r="F18" s="5"/>
+    </row>
+    <row r="19" spans="5:6">
       <c r="E19" s="5"/>
-    </row>
-    <row r="20" spans="5:5">
+      <c r="F19" s="5"/>
+    </row>
+    <row r="20" spans="5:6">
       <c r="E20" s="5"/>
-    </row>
-    <row r="21" spans="5:5">
+      <c r="F20" s="5"/>
+    </row>
+    <row r="21" spans="5:6">
       <c r="E21" s="5"/>
-    </row>
-    <row r="22" spans="5:5">
+      <c r="F21" s="5"/>
+    </row>
+    <row r="22" spans="5:6">
       <c r="E22" s="5"/>
-    </row>
-    <row r="23" spans="5:5">
+      <c r="F22" s="5"/>
+    </row>
+    <row r="23" spans="5:6">
       <c r="E23" s="5"/>
-    </row>
-    <row r="24" spans="5:5">
+      <c r="F23" s="5"/>
+    </row>
+    <row r="24" spans="5:6">
       <c r="E24" s="5"/>
-    </row>
-    <row r="25" spans="5:5">
+      <c r="F24" s="5"/>
+    </row>
+    <row r="25" spans="5:6">
       <c r="E25" s="5"/>
-    </row>
-    <row r="26" spans="5:5">
+      <c r="F25" s="5"/>
+    </row>
+    <row r="26" spans="5:6">
       <c r="E26" s="5"/>
-    </row>
-    <row r="27" spans="5:5">
+      <c r="F26" s="5"/>
+    </row>
+    <row r="27" spans="5:6">
       <c r="E27" s="5"/>
-    </row>
-    <row r="28" spans="5:5">
+      <c r="F27" s="5"/>
+    </row>
+    <row r="28" spans="5:6">
       <c r="E28" s="5"/>
-    </row>
-    <row r="29" spans="5:5">
+      <c r="F28" s="5"/>
+    </row>
+    <row r="29" spans="5:6">
       <c r="E29" s="5"/>
+      <c r="F29" s="5"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:H13" xr:uid="{30F64046-9FAB-4BA1-AF8F-52353D1AAE75}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E13">
-    <sortCondition ref="B2:B13"/>
-    <sortCondition ref="D2:D13"/>
-    <sortCondition ref="E2:E13"/>
-    <sortCondition ref="A2:A13"/>
-  </sortState>
+  <autoFilter ref="A1:I13" xr:uid="{30F64046-9FAB-4BA1-AF8F-52353D1AAE75}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -1051,7 +1108,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{21C572CC-F93B-43EE-89A4-E9C581F676FC}">
   <dimension ref="A1:E19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
make code do the lowercase comparisons, no need to LC the spreadsheet
</commit_message>
<xml_diff>
--- a/ReadAmazonKindleList/example_KindleBooks_Favorites.xlsx
+++ b/ReadAmazonKindleList/example_KindleBooks_Favorites.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub-Mark-MDO47\MDOpythonUtils\ReadAmazonKindleList\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7CED161D-0426-4E69-8A9A-93E6433CDD1E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5302D90E-4C01-4D8A-870F-0AB17EA7C952}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8415" yWindow="4560" windowWidth="28800" windowHeight="10545" xr2:uid="{0BC05AE5-A058-4C1D-AAC0-1427022E5248}"/>
+    <workbookView xWindow="2520" yWindow="4680" windowWidth="35880" windowHeight="10545" activeTab="1" xr2:uid="{0BC05AE5-A058-4C1D-AAC0-1427022E5248}"/>
   </bookViews>
   <sheets>
     <sheet name="Books" sheetId="4" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="57">
   <si>
     <t>Title</t>
   </si>
@@ -167,18 +167,6 @@
     <t>re-check</t>
   </si>
   <si>
-    <t>the history of herodotus — volume 1</t>
-  </si>
-  <si>
-    <t>the history of herodotus — volume 2</t>
-  </si>
-  <si>
-    <t>spacers</t>
-  </si>
-  <si>
-    <t>spacers: free space</t>
-  </si>
-  <si>
     <t>a</t>
   </si>
   <si>
@@ -188,25 +176,31 @@
     <t>c</t>
   </si>
   <si>
-    <t>book one of the long price quartet</t>
-  </si>
-  <si>
-    <t>book one of the slagmaster cycles</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Long Price Quartet</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Slagmaster Cycles</t>
-  </si>
-  <si>
     <t># special cases. Believe it or not, there are a bunch of normal cases too...</t>
   </si>
   <si>
-    <t># [lcstring, series, seriesNum</t>
-  </si>
-  <si>
     <t>DateAcq</t>
+  </si>
+  <si>
+    <t>The history of Herodotus — Volume 1</t>
+  </si>
+  <si>
+    <t>The history of Herodotus — Volume 2</t>
+  </si>
+  <si>
+    <t>Book One of The Long Price Quartet</t>
+  </si>
+  <si>
+    <t>Book One of The Slagmaster Cycles</t>
+  </si>
+  <si>
+    <t># [string, series, seriesNum</t>
+  </si>
+  <si>
+    <t># upper/lower case for string is ignored</t>
+  </si>
+  <si>
+    <t>Slagmaster Cycles</t>
   </si>
 </sst>
 </file>
@@ -214,7 +208,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="mm/dd/yy;@"/>
+    <numFmt numFmtId="164" formatCode="mm/dd/yy;@"/>
   </numFmts>
   <fonts count="4">
     <font>
@@ -306,7 +300,7 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Check Cell" xfId="1" builtinId="23"/>
@@ -624,7 +618,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{10CDE8BA-1414-4B51-8A6F-644E810BC2AB}">
   <dimension ref="A1:I29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="D20" sqref="D20"/>
     </sheetView>
@@ -656,7 +650,7 @@
         <v>3</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>58</v>
+        <v>49</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>34</v>
@@ -964,8 +958,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DA8C6A36-94C2-4C7F-8CA3-6F5CB9421129}">
   <dimension ref="A1:E26"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:C26"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -977,21 +971,21 @@
   <sheetData>
     <row r="1" spans="1:5" ht="16.5" thickTop="1" thickBot="1">
       <c r="A1" s="1" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>56</v>
+        <v>48</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="15.75" thickTop="1">
       <c r="A2" s="2" t="s">
-        <v>45</v>
+        <v>50</v>
       </c>
       <c r="B2" t="s">
         <v>43</v>
@@ -1000,12 +994,12 @@
         <v>1</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
     </row>
     <row r="3" spans="1:5">
       <c r="A3" s="2" t="s">
-        <v>46</v>
+        <v>51</v>
       </c>
       <c r="B3" t="s">
         <v>43</v>
@@ -1013,10 +1007,13 @@
       <c r="C3" s="5">
         <v>2</v>
       </c>
+      <c r="E3" s="4" t="s">
+        <v>55</v>
+      </c>
     </row>
     <row r="4" spans="1:5">
       <c r="A4" s="2" t="s">
-        <v>47</v>
+        <v>19</v>
       </c>
       <c r="B4" t="s">
         <v>19</v>
@@ -1027,7 +1024,7 @@
     </row>
     <row r="5" spans="1:5">
       <c r="A5" s="2" t="s">
-        <v>48</v>
+        <v>21</v>
       </c>
       <c r="B5" t="s">
         <v>19</v>
@@ -1109,7 +1106,7 @@
   <dimension ref="A1:E19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H15" sqref="H15"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1121,16 +1118,16 @@
   <sheetData>
     <row r="1" spans="1:5" ht="16.5" thickTop="1" thickBot="1">
       <c r="A1" s="1" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>56</v>
+        <v>48</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="15.75" thickTop="1">
@@ -1138,13 +1135,13 @@
         <v>52</v>
       </c>
       <c r="B2" t="s">
-        <v>54</v>
+        <v>42</v>
       </c>
       <c r="C2" s="5">
         <v>1</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -1152,10 +1149,13 @@
         <v>53</v>
       </c>
       <c r="B3" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="C3" s="5">
         <v>1</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="4" spans="1:5">

</xml_diff>

<commit_message>
add SUBSTITUTE_goofy tab to get rid of weird characters
</commit_message>
<xml_diff>
--- a/ReadAmazonKindleList/example_KindleBooks_Favorites.xlsx
+++ b/ReadAmazonKindleList/example_KindleBooks_Favorites.xlsx
@@ -1,21 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23426"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub-Mark-MDO47\MDOpythonUtils\ReadAmazonKindleList\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5302D90E-4C01-4D8A-870F-0AB17EA7C952}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51793DAE-C665-4BF9-8B54-664F98053810}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2520" yWindow="4680" windowWidth="35880" windowHeight="10545" activeTab="1" xr2:uid="{0BC05AE5-A058-4C1D-AAC0-1427022E5248}"/>
+    <workbookView xWindow="1605" yWindow="4605" windowWidth="34785" windowHeight="15360" activeTab="3" xr2:uid="{0BC05AE5-A058-4C1D-AAC0-1427022E5248}"/>
   </bookViews>
   <sheets>
     <sheet name="Books" sheetId="4" r:id="rId1"/>
     <sheet name="TITLE_totalMatch" sheetId="8" r:id="rId2"/>
     <sheet name="TITLE_partialMatch" sheetId="9" r:id="rId3"/>
+    <sheet name="SUBSTITUTE_goofy" sheetId="10" r:id="rId4"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Books!$A$1:$I$13</definedName>
@@ -30,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="70">
   <si>
     <t>Title</t>
   </si>
@@ -201,6 +202,45 @@
   </si>
   <si>
     <t>Slagmaster Cycles</t>
+  </si>
+  <si>
+    <t>â€¦</t>
+  </si>
+  <si>
+    <t>…</t>
+  </si>
+  <si>
+    <t>â€“</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>â€”</t>
+  </si>
+  <si>
+    <t>â€™</t>
+  </si>
+  <si>
+    <t>’</t>
+  </si>
+  <si>
+    <t>Ã©</t>
+  </si>
+  <si>
+    <t>é</t>
+  </si>
+  <si>
+    <t>Ã¼</t>
+  </si>
+  <si>
+    <t>ü</t>
+  </si>
+  <si>
+    <t>–</t>
+  </si>
+  <si>
+    <t>—</t>
   </si>
 </sst>
 </file>
@@ -958,7 +998,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DA8C6A36-94C2-4C7F-8CA3-6F5CB9421129}">
   <dimension ref="A1:E26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
@@ -1209,4 +1249,910 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{085F125C-4738-4BCE-BC1D-0FB9860CFA01}">
+  <dimension ref="A1:C199"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B1" t="s">
+        <v>46</v>
+      </c>
+      <c r="C1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="C2">
+        <f>LEN(A2)</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="C3">
+        <f>LEN(A3)</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="C4">
+        <f>LEN(A4)</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="C5">
+        <f>LEN(A5)</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="C6">
+        <f>LEN(A6)</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="A7" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="C7">
+        <f>LEN(A7)</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
+      <c r="A8" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="C8">
+        <f>LEN(A8)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
+      <c r="A9" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="C9">
+        <f>LEN(A9)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3">
+      <c r="A10" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="C10">
+        <f>LEN(A10)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3">
+      <c r="A11" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="C11">
+        <f>LEN(A11)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3">
+      <c r="A12" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="C12">
+        <f>LEN(A12)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3">
+      <c r="A13" s="5"/>
+      <c r="B13" s="5"/>
+    </row>
+    <row r="14" spans="1:3">
+      <c r="A14" s="5"/>
+      <c r="B14" s="5"/>
+    </row>
+    <row r="15" spans="1:3">
+      <c r="A15" s="5"/>
+      <c r="B15" s="5"/>
+    </row>
+    <row r="16" spans="1:3">
+      <c r="A16" s="5"/>
+      <c r="B16" s="5"/>
+    </row>
+    <row r="17" spans="1:2">
+      <c r="A17" s="5"/>
+      <c r="B17" s="5"/>
+    </row>
+    <row r="18" spans="1:2">
+      <c r="A18" s="5"/>
+      <c r="B18" s="5"/>
+    </row>
+    <row r="19" spans="1:2">
+      <c r="A19" s="5"/>
+      <c r="B19" s="5"/>
+    </row>
+    <row r="20" spans="1:2">
+      <c r="A20" s="5"/>
+      <c r="B20" s="5"/>
+    </row>
+    <row r="21" spans="1:2">
+      <c r="A21" s="5"/>
+      <c r="B21" s="5"/>
+    </row>
+    <row r="22" spans="1:2">
+      <c r="A22" s="5"/>
+      <c r="B22" s="5"/>
+    </row>
+    <row r="23" spans="1:2">
+      <c r="A23" s="5"/>
+      <c r="B23" s="5"/>
+    </row>
+    <row r="24" spans="1:2">
+      <c r="A24" s="5"/>
+      <c r="B24" s="5"/>
+    </row>
+    <row r="25" spans="1:2">
+      <c r="A25" s="5"/>
+      <c r="B25" s="5"/>
+    </row>
+    <row r="26" spans="1:2">
+      <c r="A26" s="5"/>
+      <c r="B26" s="5"/>
+    </row>
+    <row r="27" spans="1:2">
+      <c r="A27" s="5"/>
+      <c r="B27" s="5"/>
+    </row>
+    <row r="28" spans="1:2">
+      <c r="A28" s="5"/>
+      <c r="B28" s="5"/>
+    </row>
+    <row r="29" spans="1:2">
+      <c r="A29" s="5"/>
+      <c r="B29" s="5"/>
+    </row>
+    <row r="30" spans="1:2">
+      <c r="A30" s="5"/>
+      <c r="B30" s="5"/>
+    </row>
+    <row r="31" spans="1:2">
+      <c r="A31" s="5"/>
+      <c r="B31" s="5"/>
+    </row>
+    <row r="32" spans="1:2">
+      <c r="A32" s="5"/>
+      <c r="B32" s="5"/>
+    </row>
+    <row r="33" spans="1:2">
+      <c r="A33" s="5"/>
+      <c r="B33" s="5"/>
+    </row>
+    <row r="34" spans="1:2">
+      <c r="A34" s="5"/>
+      <c r="B34" s="5"/>
+    </row>
+    <row r="35" spans="1:2">
+      <c r="A35" s="5"/>
+      <c r="B35" s="5"/>
+    </row>
+    <row r="36" spans="1:2">
+      <c r="A36" s="5"/>
+      <c r="B36" s="5"/>
+    </row>
+    <row r="37" spans="1:2">
+      <c r="A37" s="5"/>
+      <c r="B37" s="5"/>
+    </row>
+    <row r="38" spans="1:2">
+      <c r="A38" s="5"/>
+      <c r="B38" s="5"/>
+    </row>
+    <row r="39" spans="1:2">
+      <c r="A39" s="5"/>
+      <c r="B39" s="5"/>
+    </row>
+    <row r="40" spans="1:2">
+      <c r="A40" s="5"/>
+      <c r="B40" s="5"/>
+    </row>
+    <row r="41" spans="1:2">
+      <c r="A41" s="5"/>
+      <c r="B41" s="5"/>
+    </row>
+    <row r="42" spans="1:2">
+      <c r="A42" s="5"/>
+      <c r="B42" s="5"/>
+    </row>
+    <row r="43" spans="1:2">
+      <c r="A43" s="5"/>
+      <c r="B43" s="5"/>
+    </row>
+    <row r="44" spans="1:2">
+      <c r="A44" s="5"/>
+      <c r="B44" s="5"/>
+    </row>
+    <row r="45" spans="1:2">
+      <c r="A45" s="5"/>
+      <c r="B45" s="5"/>
+    </row>
+    <row r="46" spans="1:2">
+      <c r="A46" s="5"/>
+      <c r="B46" s="5"/>
+    </row>
+    <row r="47" spans="1:2">
+      <c r="A47" s="5"/>
+      <c r="B47" s="5"/>
+    </row>
+    <row r="48" spans="1:2">
+      <c r="A48" s="5"/>
+      <c r="B48" s="5"/>
+    </row>
+    <row r="49" spans="1:2">
+      <c r="A49" s="5"/>
+      <c r="B49" s="5"/>
+    </row>
+    <row r="50" spans="1:2">
+      <c r="A50" s="5"/>
+      <c r="B50" s="5"/>
+    </row>
+    <row r="51" spans="1:2">
+      <c r="A51" s="5"/>
+      <c r="B51" s="5"/>
+    </row>
+    <row r="52" spans="1:2">
+      <c r="A52" s="5"/>
+      <c r="B52" s="5"/>
+    </row>
+    <row r="53" spans="1:2">
+      <c r="A53" s="5"/>
+      <c r="B53" s="5"/>
+    </row>
+    <row r="54" spans="1:2">
+      <c r="A54" s="5"/>
+      <c r="B54" s="5"/>
+    </row>
+    <row r="55" spans="1:2">
+      <c r="A55" s="5"/>
+      <c r="B55" s="5"/>
+    </row>
+    <row r="56" spans="1:2">
+      <c r="A56" s="5"/>
+      <c r="B56" s="5"/>
+    </row>
+    <row r="57" spans="1:2">
+      <c r="A57" s="5"/>
+      <c r="B57" s="5"/>
+    </row>
+    <row r="58" spans="1:2">
+      <c r="A58" s="5"/>
+      <c r="B58" s="5"/>
+    </row>
+    <row r="59" spans="1:2">
+      <c r="A59" s="5"/>
+      <c r="B59" s="5"/>
+    </row>
+    <row r="60" spans="1:2">
+      <c r="A60" s="5"/>
+      <c r="B60" s="5"/>
+    </row>
+    <row r="61" spans="1:2">
+      <c r="A61" s="5"/>
+      <c r="B61" s="5"/>
+    </row>
+    <row r="62" spans="1:2">
+      <c r="A62" s="5"/>
+      <c r="B62" s="5"/>
+    </row>
+    <row r="63" spans="1:2">
+      <c r="A63" s="5"/>
+      <c r="B63" s="5"/>
+    </row>
+    <row r="64" spans="1:2">
+      <c r="A64" s="5"/>
+      <c r="B64" s="5"/>
+    </row>
+    <row r="65" spans="1:2">
+      <c r="A65" s="5"/>
+      <c r="B65" s="5"/>
+    </row>
+    <row r="66" spans="1:2">
+      <c r="A66" s="5"/>
+      <c r="B66" s="5"/>
+    </row>
+    <row r="67" spans="1:2">
+      <c r="A67" s="5"/>
+      <c r="B67" s="5"/>
+    </row>
+    <row r="68" spans="1:2">
+      <c r="A68" s="5"/>
+      <c r="B68" s="5"/>
+    </row>
+    <row r="69" spans="1:2">
+      <c r="A69" s="5"/>
+      <c r="B69" s="5"/>
+    </row>
+    <row r="70" spans="1:2">
+      <c r="A70" s="5"/>
+      <c r="B70" s="5"/>
+    </row>
+    <row r="71" spans="1:2">
+      <c r="A71" s="5"/>
+      <c r="B71" s="5"/>
+    </row>
+    <row r="72" spans="1:2">
+      <c r="A72" s="5"/>
+      <c r="B72" s="5"/>
+    </row>
+    <row r="73" spans="1:2">
+      <c r="A73" s="5"/>
+      <c r="B73" s="5"/>
+    </row>
+    <row r="74" spans="1:2">
+      <c r="A74" s="5"/>
+      <c r="B74" s="5"/>
+    </row>
+    <row r="75" spans="1:2">
+      <c r="A75" s="5"/>
+      <c r="B75" s="5"/>
+    </row>
+    <row r="76" spans="1:2">
+      <c r="A76" s="5"/>
+      <c r="B76" s="5"/>
+    </row>
+    <row r="77" spans="1:2">
+      <c r="A77" s="5"/>
+      <c r="B77" s="5"/>
+    </row>
+    <row r="78" spans="1:2">
+      <c r="A78" s="5"/>
+      <c r="B78" s="5"/>
+    </row>
+    <row r="79" spans="1:2">
+      <c r="A79" s="5"/>
+      <c r="B79" s="5"/>
+    </row>
+    <row r="80" spans="1:2">
+      <c r="A80" s="5"/>
+      <c r="B80" s="5"/>
+    </row>
+    <row r="81" spans="1:2">
+      <c r="A81" s="5"/>
+      <c r="B81" s="5"/>
+    </row>
+    <row r="82" spans="1:2">
+      <c r="A82" s="5"/>
+      <c r="B82" s="5"/>
+    </row>
+    <row r="83" spans="1:2">
+      <c r="A83" s="5"/>
+      <c r="B83" s="5"/>
+    </row>
+    <row r="84" spans="1:2">
+      <c r="A84" s="5"/>
+      <c r="B84" s="5"/>
+    </row>
+    <row r="85" spans="1:2">
+      <c r="A85" s="5"/>
+      <c r="B85" s="5"/>
+    </row>
+    <row r="86" spans="1:2">
+      <c r="A86" s="5"/>
+      <c r="B86" s="5"/>
+    </row>
+    <row r="87" spans="1:2">
+      <c r="A87" s="5"/>
+      <c r="B87" s="5"/>
+    </row>
+    <row r="88" spans="1:2">
+      <c r="A88" s="5"/>
+      <c r="B88" s="5"/>
+    </row>
+    <row r="89" spans="1:2">
+      <c r="A89" s="5"/>
+      <c r="B89" s="5"/>
+    </row>
+    <row r="90" spans="1:2">
+      <c r="A90" s="5"/>
+      <c r="B90" s="5"/>
+    </row>
+    <row r="91" spans="1:2">
+      <c r="A91" s="5"/>
+      <c r="B91" s="5"/>
+    </row>
+    <row r="92" spans="1:2">
+      <c r="A92" s="5"/>
+      <c r="B92" s="5"/>
+    </row>
+    <row r="93" spans="1:2">
+      <c r="A93" s="5"/>
+      <c r="B93" s="5"/>
+    </row>
+    <row r="94" spans="1:2">
+      <c r="A94" s="5"/>
+      <c r="B94" s="5"/>
+    </row>
+    <row r="95" spans="1:2">
+      <c r="A95" s="5"/>
+      <c r="B95" s="5"/>
+    </row>
+    <row r="96" spans="1:2">
+      <c r="A96" s="5"/>
+      <c r="B96" s="5"/>
+    </row>
+    <row r="97" spans="1:2">
+      <c r="A97" s="5"/>
+      <c r="B97" s="5"/>
+    </row>
+    <row r="98" spans="1:2">
+      <c r="A98" s="5"/>
+      <c r="B98" s="5"/>
+    </row>
+    <row r="99" spans="1:2">
+      <c r="A99" s="5"/>
+      <c r="B99" s="5"/>
+    </row>
+    <row r="100" spans="1:2">
+      <c r="A100" s="5"/>
+      <c r="B100" s="5"/>
+    </row>
+    <row r="101" spans="1:2">
+      <c r="A101" s="5"/>
+      <c r="B101" s="5"/>
+    </row>
+    <row r="102" spans="1:2">
+      <c r="A102" s="5"/>
+      <c r="B102" s="5"/>
+    </row>
+    <row r="103" spans="1:2">
+      <c r="A103" s="5"/>
+      <c r="B103" s="5"/>
+    </row>
+    <row r="104" spans="1:2">
+      <c r="A104" s="5"/>
+      <c r="B104" s="5"/>
+    </row>
+    <row r="105" spans="1:2">
+      <c r="A105" s="5"/>
+      <c r="B105" s="5"/>
+    </row>
+    <row r="106" spans="1:2">
+      <c r="A106" s="5"/>
+      <c r="B106" s="5"/>
+    </row>
+    <row r="107" spans="1:2">
+      <c r="A107" s="5"/>
+      <c r="B107" s="5"/>
+    </row>
+    <row r="108" spans="1:2">
+      <c r="A108" s="5"/>
+      <c r="B108" s="5"/>
+    </row>
+    <row r="109" spans="1:2">
+      <c r="A109" s="5"/>
+      <c r="B109" s="5"/>
+    </row>
+    <row r="110" spans="1:2">
+      <c r="A110" s="5"/>
+      <c r="B110" s="5"/>
+    </row>
+    <row r="111" spans="1:2">
+      <c r="A111" s="5"/>
+      <c r="B111" s="5"/>
+    </row>
+    <row r="112" spans="1:2">
+      <c r="A112" s="5"/>
+      <c r="B112" s="5"/>
+    </row>
+    <row r="113" spans="1:2">
+      <c r="A113" s="5"/>
+      <c r="B113" s="5"/>
+    </row>
+    <row r="114" spans="1:2">
+      <c r="A114" s="5"/>
+      <c r="B114" s="5"/>
+    </row>
+    <row r="115" spans="1:2">
+      <c r="A115" s="5"/>
+      <c r="B115" s="5"/>
+    </row>
+    <row r="116" spans="1:2">
+      <c r="A116" s="5"/>
+      <c r="B116" s="5"/>
+    </row>
+    <row r="117" spans="1:2">
+      <c r="A117" s="5"/>
+      <c r="B117" s="5"/>
+    </row>
+    <row r="118" spans="1:2">
+      <c r="A118" s="5"/>
+      <c r="B118" s="5"/>
+    </row>
+    <row r="119" spans="1:2">
+      <c r="A119" s="5"/>
+      <c r="B119" s="5"/>
+    </row>
+    <row r="120" spans="1:2">
+      <c r="A120" s="5"/>
+      <c r="B120" s="5"/>
+    </row>
+    <row r="121" spans="1:2">
+      <c r="A121" s="5"/>
+      <c r="B121" s="5"/>
+    </row>
+    <row r="122" spans="1:2">
+      <c r="A122" s="5"/>
+      <c r="B122" s="5"/>
+    </row>
+    <row r="123" spans="1:2">
+      <c r="A123" s="5"/>
+      <c r="B123" s="5"/>
+    </row>
+    <row r="124" spans="1:2">
+      <c r="A124" s="5"/>
+      <c r="B124" s="5"/>
+    </row>
+    <row r="125" spans="1:2">
+      <c r="A125" s="5"/>
+      <c r="B125" s="5"/>
+    </row>
+    <row r="126" spans="1:2">
+      <c r="A126" s="5"/>
+      <c r="B126" s="5"/>
+    </row>
+    <row r="127" spans="1:2">
+      <c r="A127" s="5"/>
+      <c r="B127" s="5"/>
+    </row>
+    <row r="128" spans="1:2">
+      <c r="A128" s="5"/>
+      <c r="B128" s="5"/>
+    </row>
+    <row r="129" spans="1:2">
+      <c r="A129" s="5"/>
+      <c r="B129" s="5"/>
+    </row>
+    <row r="130" spans="1:2">
+      <c r="A130" s="5"/>
+      <c r="B130" s="5"/>
+    </row>
+    <row r="131" spans="1:2">
+      <c r="A131" s="5"/>
+      <c r="B131" s="5"/>
+    </row>
+    <row r="132" spans="1:2">
+      <c r="A132" s="5"/>
+      <c r="B132" s="5"/>
+    </row>
+    <row r="133" spans="1:2">
+      <c r="A133" s="5"/>
+      <c r="B133" s="5"/>
+    </row>
+    <row r="134" spans="1:2">
+      <c r="A134" s="5"/>
+      <c r="B134" s="5"/>
+    </row>
+    <row r="135" spans="1:2">
+      <c r="A135" s="5"/>
+      <c r="B135" s="5"/>
+    </row>
+    <row r="136" spans="1:2">
+      <c r="A136" s="5"/>
+      <c r="B136" s="5"/>
+    </row>
+    <row r="137" spans="1:2">
+      <c r="A137" s="5"/>
+      <c r="B137" s="5"/>
+    </row>
+    <row r="138" spans="1:2">
+      <c r="A138" s="5"/>
+      <c r="B138" s="5"/>
+    </row>
+    <row r="139" spans="1:2">
+      <c r="A139" s="5"/>
+      <c r="B139" s="5"/>
+    </row>
+    <row r="140" spans="1:2">
+      <c r="A140" s="5"/>
+      <c r="B140" s="5"/>
+    </row>
+    <row r="141" spans="1:2">
+      <c r="A141" s="5"/>
+      <c r="B141" s="5"/>
+    </row>
+    <row r="142" spans="1:2">
+      <c r="A142" s="5"/>
+      <c r="B142" s="5"/>
+    </row>
+    <row r="143" spans="1:2">
+      <c r="A143" s="5"/>
+      <c r="B143" s="5"/>
+    </row>
+    <row r="144" spans="1:2">
+      <c r="A144" s="5"/>
+      <c r="B144" s="5"/>
+    </row>
+    <row r="145" spans="1:2">
+      <c r="A145" s="5"/>
+      <c r="B145" s="5"/>
+    </row>
+    <row r="146" spans="1:2">
+      <c r="A146" s="5"/>
+      <c r="B146" s="5"/>
+    </row>
+    <row r="147" spans="1:2">
+      <c r="A147" s="5"/>
+      <c r="B147" s="5"/>
+    </row>
+    <row r="148" spans="1:2">
+      <c r="A148" s="5"/>
+      <c r="B148" s="5"/>
+    </row>
+    <row r="149" spans="1:2">
+      <c r="A149" s="5"/>
+      <c r="B149" s="5"/>
+    </row>
+    <row r="150" spans="1:2">
+      <c r="A150" s="5"/>
+      <c r="B150" s="5"/>
+    </row>
+    <row r="151" spans="1:2">
+      <c r="A151" s="5"/>
+      <c r="B151" s="5"/>
+    </row>
+    <row r="152" spans="1:2">
+      <c r="A152" s="5"/>
+      <c r="B152" s="5"/>
+    </row>
+    <row r="153" spans="1:2">
+      <c r="A153" s="5"/>
+      <c r="B153" s="5"/>
+    </row>
+    <row r="154" spans="1:2">
+      <c r="A154" s="5"/>
+      <c r="B154" s="5"/>
+    </row>
+    <row r="155" spans="1:2">
+      <c r="A155" s="5"/>
+      <c r="B155" s="5"/>
+    </row>
+    <row r="156" spans="1:2">
+      <c r="A156" s="5"/>
+      <c r="B156" s="5"/>
+    </row>
+    <row r="157" spans="1:2">
+      <c r="A157" s="5"/>
+      <c r="B157" s="5"/>
+    </row>
+    <row r="158" spans="1:2">
+      <c r="A158" s="5"/>
+      <c r="B158" s="5"/>
+    </row>
+    <row r="159" spans="1:2">
+      <c r="A159" s="5"/>
+      <c r="B159" s="5"/>
+    </row>
+    <row r="160" spans="1:2">
+      <c r="A160" s="5"/>
+      <c r="B160" s="5"/>
+    </row>
+    <row r="161" spans="1:2">
+      <c r="A161" s="5"/>
+      <c r="B161" s="5"/>
+    </row>
+    <row r="162" spans="1:2">
+      <c r="A162" s="5"/>
+      <c r="B162" s="5"/>
+    </row>
+    <row r="163" spans="1:2">
+      <c r="A163" s="5"/>
+      <c r="B163" s="5"/>
+    </row>
+    <row r="164" spans="1:2">
+      <c r="A164" s="5"/>
+      <c r="B164" s="5"/>
+    </row>
+    <row r="165" spans="1:2">
+      <c r="A165" s="5"/>
+      <c r="B165" s="5"/>
+    </row>
+    <row r="166" spans="1:2">
+      <c r="A166" s="5"/>
+      <c r="B166" s="5"/>
+    </row>
+    <row r="167" spans="1:2">
+      <c r="A167" s="5"/>
+      <c r="B167" s="5"/>
+    </row>
+    <row r="168" spans="1:2">
+      <c r="A168" s="5"/>
+      <c r="B168" s="5"/>
+    </row>
+    <row r="169" spans="1:2">
+      <c r="A169" s="5"/>
+      <c r="B169" s="5"/>
+    </row>
+    <row r="170" spans="1:2">
+      <c r="A170" s="5"/>
+      <c r="B170" s="5"/>
+    </row>
+    <row r="171" spans="1:2">
+      <c r="A171" s="5"/>
+      <c r="B171" s="5"/>
+    </row>
+    <row r="172" spans="1:2">
+      <c r="A172" s="5"/>
+      <c r="B172" s="5"/>
+    </row>
+    <row r="173" spans="1:2">
+      <c r="A173" s="5"/>
+      <c r="B173" s="5"/>
+    </row>
+    <row r="174" spans="1:2">
+      <c r="A174" s="5"/>
+      <c r="B174" s="5"/>
+    </row>
+    <row r="175" spans="1:2">
+      <c r="A175" s="5"/>
+      <c r="B175" s="5"/>
+    </row>
+    <row r="176" spans="1:2">
+      <c r="A176" s="5"/>
+      <c r="B176" s="5"/>
+    </row>
+    <row r="177" spans="1:2">
+      <c r="A177" s="5"/>
+      <c r="B177" s="5"/>
+    </row>
+    <row r="178" spans="1:2">
+      <c r="A178" s="5"/>
+      <c r="B178" s="5"/>
+    </row>
+    <row r="179" spans="1:2">
+      <c r="A179" s="5"/>
+      <c r="B179" s="5"/>
+    </row>
+    <row r="180" spans="1:2">
+      <c r="A180" s="5"/>
+      <c r="B180" s="5"/>
+    </row>
+    <row r="181" spans="1:2">
+      <c r="A181" s="5"/>
+      <c r="B181" s="5"/>
+    </row>
+    <row r="182" spans="1:2">
+      <c r="A182" s="5"/>
+      <c r="B182" s="5"/>
+    </row>
+    <row r="183" spans="1:2">
+      <c r="A183" s="5"/>
+      <c r="B183" s="5"/>
+    </row>
+    <row r="184" spans="1:2">
+      <c r="A184" s="5"/>
+      <c r="B184" s="5"/>
+    </row>
+    <row r="185" spans="1:2">
+      <c r="A185" s="5"/>
+      <c r="B185" s="5"/>
+    </row>
+    <row r="186" spans="1:2">
+      <c r="A186" s="5"/>
+      <c r="B186" s="5"/>
+    </row>
+    <row r="187" spans="1:2">
+      <c r="A187" s="5"/>
+      <c r="B187" s="5"/>
+    </row>
+    <row r="188" spans="1:2">
+      <c r="A188" s="5"/>
+      <c r="B188" s="5"/>
+    </row>
+    <row r="189" spans="1:2">
+      <c r="A189" s="5"/>
+      <c r="B189" s="5"/>
+    </row>
+    <row r="190" spans="1:2">
+      <c r="A190" s="5"/>
+      <c r="B190" s="5"/>
+    </row>
+    <row r="191" spans="1:2">
+      <c r="A191" s="5"/>
+      <c r="B191" s="5"/>
+    </row>
+    <row r="192" spans="1:2">
+      <c r="A192" s="5"/>
+      <c r="B192" s="5"/>
+    </row>
+    <row r="193" spans="1:2">
+      <c r="A193" s="5"/>
+      <c r="B193" s="5"/>
+    </row>
+    <row r="194" spans="1:2">
+      <c r="A194" s="5"/>
+      <c r="B194" s="5"/>
+    </row>
+    <row r="195" spans="1:2">
+      <c r="A195" s="5"/>
+      <c r="B195" s="5"/>
+    </row>
+    <row r="196" spans="1:2">
+      <c r="A196" s="5"/>
+      <c r="B196" s="5"/>
+    </row>
+    <row r="197" spans="1:2">
+      <c r="A197" s="5"/>
+      <c r="B197" s="5"/>
+    </row>
+    <row r="198" spans="1:2">
+      <c r="A198" s="5"/>
+      <c r="B198" s="5"/>
+    </row>
+    <row r="199" spans="1:2">
+      <c r="A199" s="5"/>
+      <c r="B199" s="5"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
handle new format of data from Amazon
</commit_message>
<xml_diff>
--- a/ReadAmazonKindleList/example_KindleBooks_Favorites.xlsx
+++ b/ReadAmazonKindleList/example_KindleBooks_Favorites.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub-Mark-MDO47\MDOpythonUtils\ReadAmazonKindleList\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51793DAE-C665-4BF9-8B54-664F98053810}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2662F270-312E-4651-BCBA-41FC54AC2630}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1605" yWindow="4605" windowWidth="34785" windowHeight="15360" activeTab="3" xr2:uid="{0BC05AE5-A058-4C1D-AAC0-1427022E5248}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21390" xr2:uid="{0BC05AE5-A058-4C1D-AAC0-1427022E5248}"/>
   </bookViews>
   <sheets>
     <sheet name="Books" sheetId="4" r:id="rId1"/>
@@ -19,7 +19,7 @@
     <sheet name="SUBSTITUTE_goofy" sheetId="10" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Books!$A$1:$I$13</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Books!$A$1:$J$13</definedName>
   </definedNames>
   <calcPr calcId="181029"/>
   <extLst>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="72">
   <si>
     <t>Title</t>
   </si>
@@ -241,6 +241,12 @@
   </si>
   <si>
     <t>—</t>
+  </si>
+  <si>
+    <t>Read</t>
+  </si>
+  <si>
+    <t>READ</t>
   </si>
 </sst>
 </file>
@@ -656,11 +662,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{10CDE8BA-1414-4B51-8A6F-644E810BC2AB}">
-  <dimension ref="A1:I29"/>
+  <dimension ref="A1:J29"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D20" sqref="D20"/>
+      <selection pane="bottomLeft" activeCell="M21" sqref="M21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -670,10 +676,11 @@
     <col min="3" max="3" width="26.28515625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="30.5703125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="7.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7.5703125" customWidth="1"/>
+    <col min="7" max="7" width="10.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="16.5" thickTop="1" thickBot="1">
+    <row r="1" spans="1:10" ht="16.5" thickTop="1" thickBot="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -690,19 +697,22 @@
         <v>3</v>
       </c>
       <c r="F1" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="15.75" thickTop="1">
+    <row r="2" spans="1:10" ht="15.75" thickTop="1">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -718,14 +728,15 @@
       <c r="E2" s="5">
         <v>1</v>
       </c>
-      <c r="F2" s="6">
+      <c r="F2" s="5"/>
+      <c r="G2" s="6">
         <v>43724</v>
       </c>
-      <c r="G2" t="s">
+      <c r="H2" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="3" spans="1:9">
+    <row r="3" spans="1:10">
       <c r="A3" t="s">
         <v>41</v>
       </c>
@@ -736,14 +747,17 @@
         <v>6</v>
       </c>
       <c r="E3" s="5"/>
-      <c r="F3" s="6">
+      <c r="F3" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="G3" s="6">
         <v>43907</v>
       </c>
-      <c r="G3" t="s">
+      <c r="H3" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="4" spans="1:9">
+    <row r="4" spans="1:10">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -759,11 +773,12 @@
       <c r="E4" s="5">
         <v>1</v>
       </c>
-      <c r="F4" s="6">
+      <c r="F4" s="5"/>
+      <c r="G4" s="6">
         <v>44010</v>
       </c>
     </row>
-    <row r="5" spans="1:9">
+    <row r="5" spans="1:10">
       <c r="A5" t="s">
         <v>9</v>
       </c>
@@ -779,11 +794,12 @@
       <c r="E5" s="5">
         <v>1</v>
       </c>
-      <c r="F5" s="6">
+      <c r="F5" s="5"/>
+      <c r="G5" s="6">
         <v>43985</v>
       </c>
     </row>
-    <row r="6" spans="1:9">
+    <row r="6" spans="1:10">
       <c r="A6" t="s">
         <v>11</v>
       </c>
@@ -794,11 +810,12 @@
         <v>12</v>
       </c>
       <c r="E6" s="5"/>
-      <c r="F6" s="6">
+      <c r="F6" s="5"/>
+      <c r="G6" s="6">
         <v>41670</v>
       </c>
     </row>
-    <row r="7" spans="1:9">
+    <row r="7" spans="1:10">
       <c r="A7" t="s">
         <v>13</v>
       </c>
@@ -809,11 +826,12 @@
         <v>14</v>
       </c>
       <c r="E7" s="5"/>
-      <c r="F7" s="6">
+      <c r="F7" s="5"/>
+      <c r="G7" s="6">
         <v>43786</v>
       </c>
     </row>
-    <row r="8" spans="1:9">
+    <row r="8" spans="1:10">
       <c r="A8" t="s">
         <v>15</v>
       </c>
@@ -824,11 +842,12 @@
         <v>16</v>
       </c>
       <c r="E8" s="5"/>
-      <c r="F8" s="6">
+      <c r="F8" s="5"/>
+      <c r="G8" s="6">
         <v>43793</v>
       </c>
     </row>
-    <row r="9" spans="1:9">
+    <row r="9" spans="1:10">
       <c r="A9" t="s">
         <v>17</v>
       </c>
@@ -839,14 +858,15 @@
         <v>18</v>
       </c>
       <c r="E9" s="5"/>
-      <c r="F9" s="6">
+      <c r="F9" s="5"/>
+      <c r="G9" s="6">
         <v>43652</v>
       </c>
-      <c r="G9" t="s">
+      <c r="H9" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="10" spans="1:9">
+    <row r="10" spans="1:10">
       <c r="A10" t="s">
         <v>19</v>
       </c>
@@ -862,11 +882,12 @@
       <c r="E10" s="5">
         <v>1</v>
       </c>
-      <c r="F10" s="6">
+      <c r="F10" s="5"/>
+      <c r="G10" s="6">
         <v>43730</v>
       </c>
     </row>
-    <row r="11" spans="1:9">
+    <row r="11" spans="1:10">
       <c r="A11" t="s">
         <v>21</v>
       </c>
@@ -882,11 +903,12 @@
       <c r="E11" s="5">
         <v>2</v>
       </c>
-      <c r="F11" s="6">
+      <c r="F11" s="5"/>
+      <c r="G11" s="6">
         <v>43723</v>
       </c>
     </row>
-    <row r="12" spans="1:9">
+    <row r="12" spans="1:10">
       <c r="A12" t="s">
         <v>24</v>
       </c>
@@ -902,11 +924,12 @@
       <c r="E12" s="5">
         <v>1</v>
       </c>
-      <c r="F12" s="6">
+      <c r="F12" s="5"/>
+      <c r="G12" s="6">
         <v>43532</v>
       </c>
     </row>
-    <row r="13" spans="1:9">
+    <row r="13" spans="1:10">
       <c r="A13" t="s">
         <v>22</v>
       </c>
@@ -917,79 +940,96 @@
         <v>23</v>
       </c>
       <c r="E13" s="5"/>
-      <c r="F13" s="6">
+      <c r="F13" s="5"/>
+      <c r="G13" s="6">
         <v>43532</v>
       </c>
-      <c r="I13" t="s">
+      <c r="J13" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="14" spans="1:9">
+    <row r="14" spans="1:10">
       <c r="E14" s="5"/>
       <c r="F14" s="5"/>
-    </row>
-    <row r="15" spans="1:9">
+      <c r="G14" s="5"/>
+    </row>
+    <row r="15" spans="1:10">
       <c r="E15" s="5"/>
       <c r="F15" s="5"/>
-    </row>
-    <row r="16" spans="1:9">
+      <c r="G15" s="5"/>
+    </row>
+    <row r="16" spans="1:10">
       <c r="E16" s="5"/>
       <c r="F16" s="5"/>
-    </row>
-    <row r="17" spans="5:6">
+      <c r="G16" s="5"/>
+    </row>
+    <row r="17" spans="5:7">
       <c r="E17" s="5"/>
       <c r="F17" s="5"/>
-    </row>
-    <row r="18" spans="5:6">
+      <c r="G17" s="5"/>
+    </row>
+    <row r="18" spans="5:7">
       <c r="E18" s="5"/>
       <c r="F18" s="5"/>
-    </row>
-    <row r="19" spans="5:6">
+      <c r="G18" s="5"/>
+    </row>
+    <row r="19" spans="5:7">
       <c r="E19" s="5"/>
       <c r="F19" s="5"/>
-    </row>
-    <row r="20" spans="5:6">
+      <c r="G19" s="5"/>
+    </row>
+    <row r="20" spans="5:7">
       <c r="E20" s="5"/>
       <c r="F20" s="5"/>
-    </row>
-    <row r="21" spans="5:6">
+      <c r="G20" s="5"/>
+    </row>
+    <row r="21" spans="5:7">
       <c r="E21" s="5"/>
       <c r="F21" s="5"/>
-    </row>
-    <row r="22" spans="5:6">
+      <c r="G21" s="5"/>
+    </row>
+    <row r="22" spans="5:7">
       <c r="E22" s="5"/>
       <c r="F22" s="5"/>
-    </row>
-    <row r="23" spans="5:6">
+      <c r="G22" s="5"/>
+    </row>
+    <row r="23" spans="5:7">
       <c r="E23" s="5"/>
       <c r="F23" s="5"/>
-    </row>
-    <row r="24" spans="5:6">
+      <c r="G23" s="5"/>
+    </row>
+    <row r="24" spans="5:7">
       <c r="E24" s="5"/>
       <c r="F24" s="5"/>
-    </row>
-    <row r="25" spans="5:6">
+      <c r="G24" s="5"/>
+    </row>
+    <row r="25" spans="5:7">
       <c r="E25" s="5"/>
       <c r="F25" s="5"/>
-    </row>
-    <row r="26" spans="5:6">
+      <c r="G25" s="5"/>
+    </row>
+    <row r="26" spans="5:7">
       <c r="E26" s="5"/>
       <c r="F26" s="5"/>
-    </row>
-    <row r="27" spans="5:6">
+      <c r="G26" s="5"/>
+    </row>
+    <row r="27" spans="5:7">
       <c r="E27" s="5"/>
       <c r="F27" s="5"/>
-    </row>
-    <row r="28" spans="5:6">
+      <c r="G27" s="5"/>
+    </row>
+    <row r="28" spans="5:7">
       <c r="E28" s="5"/>
       <c r="F28" s="5"/>
-    </row>
-    <row r="29" spans="5:6">
+      <c r="G28" s="5"/>
+    </row>
+    <row r="29" spans="5:7">
       <c r="E29" s="5"/>
       <c r="F29" s="5"/>
+      <c r="G29" s="5"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:I13" xr:uid="{30F64046-9FAB-4BA1-AF8F-52353D1AAE75}"/>
+  <autoFilter ref="A1:J13" xr:uid="{30F64046-9FAB-4BA1-AF8F-52353D1AAE75}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -1255,7 +1295,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{085F125C-4738-4BCE-BC1D-0FB9860CFA01}">
   <dimension ref="A1:C199"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
@@ -1280,7 +1320,7 @@
         <v>58</v>
       </c>
       <c r="C2">
-        <f>LEN(A2)</f>
+        <f t="shared" ref="C2:C12" si="0">LEN(A2)</f>
         <v>3</v>
       </c>
     </row>
@@ -1292,7 +1332,7 @@
         <v>60</v>
       </c>
       <c r="C3">
-        <f>LEN(A3)</f>
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
     </row>
@@ -1304,7 +1344,7 @@
         <v>60</v>
       </c>
       <c r="C4">
-        <f>LEN(A4)</f>
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
     </row>
@@ -1316,7 +1356,7 @@
         <v>63</v>
       </c>
       <c r="C5">
-        <f>LEN(A5)</f>
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
     </row>
@@ -1328,7 +1368,7 @@
         <v>65</v>
       </c>
       <c r="C6">
-        <f>LEN(A6)</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
     </row>
@@ -1340,7 +1380,7 @@
         <v>67</v>
       </c>
       <c r="C7">
-        <f>LEN(A7)</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
     </row>
@@ -1352,7 +1392,7 @@
         <v>60</v>
       </c>
       <c r="C8">
-        <f>LEN(A8)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -1364,7 +1404,7 @@
         <v>60</v>
       </c>
       <c r="C9">
-        <f>LEN(A9)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -1376,7 +1416,7 @@
         <v>60</v>
       </c>
       <c r="C10">
-        <f>LEN(A10)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -1388,7 +1428,7 @@
         <v>60</v>
       </c>
       <c r="C11">
-        <f>LEN(A11)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -1400,7 +1440,7 @@
         <v>58</v>
       </c>
       <c r="C12">
-        <f>LEN(A12)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>

</xml_diff>